<commit_message>
Updated files for publishing
</commit_message>
<xml_diff>
--- a/Sources for elasticities.xlsx
+++ b/Sources for elasticities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jryter_usgs_gov/Documents/Documents/generalizationOutside/generalization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jryter_usgs_gov/Documents/Documents/generalizationOutside/GLOMBO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{E6019A56-43EB-BB42-BA89-4D38BB8290A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA8FEC48-683A-4632-8112-3396AC67709E}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{E6019A56-43EB-BB42-BA89-4D38BB8290A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E4554DA-D320-4A6A-B1DC-4F27A014AF14}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EB28900-207C-9445-B75A-4B376A4483BE}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{2EB28900-207C-9445-B75A-4B376A4483BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5828" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5822" uniqueCount="860">
   <si>
     <t>Demand elasticity to price</t>
   </si>
@@ -2643,6 +2643,9 @@
   </si>
   <si>
     <t>Rest of world</t>
+  </si>
+  <si>
+    <t>Hard to tell how many regressors were actually used</t>
   </si>
 </sst>
 </file>
@@ -3188,11 +3191,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FEA820-6AE6-CD42-B2A0-D4633FE287BB}">
   <dimension ref="A1:T733"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G28" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView tabSelected="1" topLeftCell="G201" workbookViewId="0">
+      <selection activeCell="Q91" sqref="Q91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="18" t="s">
@@ -3298,9 +3301,7 @@
       <c r="Q2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="18" t="s">
-        <v>793</v>
-      </c>
+      <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="18" t="s">
@@ -6373,9 +6374,7 @@
       <c r="Q78" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="R78" s="18" t="s">
-        <v>70</v>
-      </c>
+      <c r="R78" s="18"/>
     </row>
     <row r="79" spans="1:20">
       <c r="A79" s="18" t="s">
@@ -6445,7 +6444,7 @@
         <v>77</v>
       </c>
       <c r="Q80" s="18" t="s">
-        <v>81</v>
+        <v>859</v>
       </c>
     </row>
     <row r="81" spans="1:20">
@@ -6657,9 +6656,7 @@
       <c r="P86" s="18" t="s">
         <v>433</v>
       </c>
-      <c r="Q86" s="18" t="s">
-        <v>434</v>
-      </c>
+      <c r="Q86" s="18"/>
       <c r="R86" s="17"/>
       <c r="S86" s="17"/>
       <c r="T86" s="17"/>
@@ -6695,9 +6692,7 @@
       <c r="P87" s="18" t="s">
         <v>433</v>
       </c>
-      <c r="Q87" s="18" t="s">
-        <v>434</v>
-      </c>
+      <c r="Q87" s="18"/>
       <c r="R87" s="17"/>
       <c r="S87" s="17"/>
       <c r="T87" s="17"/>
@@ -6835,9 +6830,7 @@
       <c r="P91" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="Q91" s="18" t="s">
-        <v>443</v>
-      </c>
+      <c r="Q91" s="18"/>
       <c r="R91" s="17"/>
       <c r="S91" s="17"/>
       <c r="T91" s="17"/>
@@ -6873,9 +6866,7 @@
       <c r="P92" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="Q92" s="18" t="s">
-        <v>443</v>
-      </c>
+      <c r="Q92" s="18"/>
       <c r="R92" s="17"/>
       <c r="S92" s="17"/>
       <c r="T92" s="17"/>
@@ -24932,13 +24923,13 @@
       <selection pane="bottomLeft" activeCell="F220" sqref="F219:N220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.875" customWidth="1"/>
+    <col min="1" max="1" width="37.34765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.84765625" customWidth="1"/>
     <col min="3" max="3" width="29.5" customWidth="1"/>
-    <col min="4" max="4" width="10.875" customWidth="1"/>
-    <col min="6" max="13" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="10.84765625" customWidth="1"/>
+    <col min="6" max="13" width="10.84765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -33229,12 +33220,12 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="10.875" style="2"/>
-    <col min="3" max="3" width="44.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="137.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.84765625" style="2"/>
+    <col min="3" max="3" width="44.09765625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.09765625" customWidth="1"/>
+    <col min="5" max="5" width="137.59765625" style="2" customWidth="1"/>
     <col min="6" max="6" width="21.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -33338,7 +33329,7 @@
       <c r="Y3" s="17"/>
       <c r="Z3" s="17"/>
     </row>
-    <row r="4" spans="1:26" ht="63">
+    <row r="4" spans="1:26" ht="62.4">
       <c r="A4" s="6" t="s">
         <v>108</v>
       </c>
@@ -33358,7 +33349,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="47.25">
+    <row r="5" spans="1:26" ht="46.8">
       <c r="A5" s="6" t="s">
         <v>107</v>
       </c>
@@ -33378,7 +33369,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="47.25">
+    <row r="6" spans="1:26" ht="46.8">
       <c r="A6" s="6" t="s">
         <v>129</v>
       </c>
@@ -33398,7 +33389,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="47.25">
+    <row r="7" spans="1:26" ht="46.8">
       <c r="A7" s="1" t="s">
         <v>157</v>
       </c>
@@ -33475,7 +33466,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="63">
+    <row r="10" spans="1:26" ht="62.4">
       <c r="A10" s="1" t="s">
         <v>176</v>
       </c>
@@ -33495,7 +33486,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="47.25">
+    <row r="11" spans="1:26" ht="46.8">
       <c r="A11" s="1" t="s">
         <v>198</v>
       </c>
@@ -33515,7 +33506,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="31.5">
+    <row r="12" spans="1:26" ht="31.2">
       <c r="A12" s="1" t="s">
         <v>153</v>
       </c>
@@ -33535,7 +33526,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="47.25">
+    <row r="13" spans="1:26" ht="31.2">
       <c r="A13" s="1" t="s">
         <v>265</v>
       </c>
@@ -33595,7 +33586,7 @@
       <c r="Y14" s="17"/>
       <c r="Z14" s="17"/>
     </row>
-    <row r="15" spans="1:26" ht="47.25">
+    <row r="15" spans="1:26" ht="46.8">
       <c r="A15" s="1" t="s">
         <v>191</v>
       </c>
@@ -33612,7 +33603,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="31.5">
+    <row r="16" spans="1:26" ht="31.2">
       <c r="A16" s="1" t="s">
         <v>211</v>
       </c>
@@ -33629,7 +33620,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="78.75">
+    <row r="17" spans="1:6" ht="78">
       <c r="A17" s="1" t="s">
         <v>148</v>
       </c>
@@ -33649,7 +33640,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="47.25">
+    <row r="18" spans="1:6" ht="46.8">
       <c r="A18" s="1" t="s">
         <v>138</v>
       </c>
@@ -33666,7 +33657,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="47.25">
+    <row r="19" spans="1:6" ht="46.8">
       <c r="A19" s="1" t="s">
         <v>141</v>
       </c>
@@ -33683,7 +33674,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="31.5">
+    <row r="20" spans="1:6" ht="31.2">
       <c r="A20" s="1" t="s">
         <v>143</v>
       </c>
@@ -33723,7 +33714,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.5">
+    <row r="22" spans="1:6" ht="31.2">
       <c r="A22" s="1" t="s">
         <v>164</v>
       </c>
@@ -33760,7 +33751,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31.5">
+    <row r="24" spans="1:6" ht="31.2">
       <c r="A24" s="1" t="s">
         <v>160</v>
       </c>
@@ -33780,7 +33771,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="47.25">
+    <row r="25" spans="1:6" ht="46.8">
       <c r="A25" s="6" t="s">
         <v>116</v>
       </c>
@@ -33800,7 +33791,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="31.5">
+    <row r="26" spans="1:6" ht="31.2">
       <c r="A26" s="1" t="s">
         <v>187</v>
       </c>
@@ -33820,7 +33811,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="31.5">
+    <row r="27" spans="1:6" ht="31.2">
       <c r="A27" s="1" t="s">
         <v>273</v>
       </c>
@@ -33840,7 +33831,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="63">
+    <row r="28" spans="1:6" ht="62.4">
       <c r="A28" s="1" t="s">
         <v>182</v>
       </c>
@@ -33860,7 +33851,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="31.5">
+    <row r="29" spans="1:6" ht="31.2">
       <c r="A29" s="6" t="s">
         <v>120</v>
       </c>
@@ -33880,7 +33871,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="63">
+    <row r="30" spans="1:6" ht="62.4">
       <c r="A30" s="1" t="s">
         <v>203</v>
       </c>
@@ -33900,7 +33891,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="47.25">
+    <row r="31" spans="1:6" ht="31.2">
       <c r="A31" s="1" t="s">
         <v>260</v>
       </c>
@@ -33920,7 +33911,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="47.25">
+    <row r="32" spans="1:6" ht="46.8">
       <c r="A32" s="1" t="s">
         <v>172</v>
       </c>
@@ -34000,7 +33991,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="31.5">
+    <row r="35" spans="1:26" ht="31.2">
       <c r="A35" s="1" t="s">
         <v>145</v>
       </c>
@@ -34092,12 +34083,12 @@
       <selection activeCell="B31" sqref="B31:M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.25">
+    <row r="1" spans="1:13" ht="23.1">
       <c r="A1" s="25" t="s">
         <v>247</v>
       </c>
@@ -35013,7 +35004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="23.25">
+    <row r="27" spans="1:13" ht="23.1">
       <c r="A27" s="25" t="s">
         <v>249</v>
       </c>
@@ -35847,12 +35838,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="20.25">
+    <row r="52" spans="1:13" ht="20.100000000000001">
       <c r="A52" s="12" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="21">
+    <row r="56" spans="1:13" ht="20.399999999999999">
       <c r="A56" s="14" t="s">
         <v>254</v>
       </c>
@@ -36016,62 +36007,62 @@
         <v>255</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18.75">
+    <row r="60" spans="1:13" ht="18.3">
       <c r="A60" s="13"/>
     </row>
-    <row r="61" spans="1:13" ht="18.75">
+    <row r="61" spans="1:13" ht="18.3">
       <c r="A61" s="13"/>
     </row>
-    <row r="62" spans="1:13" ht="18.75">
+    <row r="62" spans="1:13" ht="18.3">
       <c r="A62" s="13"/>
     </row>
-    <row r="63" spans="1:13" ht="18.75">
+    <row r="63" spans="1:13" ht="18.3">
       <c r="A63" s="13"/>
     </row>
-    <row r="64" spans="1:13" ht="18.75">
+    <row r="64" spans="1:13" ht="18.3">
       <c r="A64" s="13"/>
     </row>
-    <row r="65" spans="1:3" ht="18.75">
+    <row r="65" spans="1:3" ht="18.3">
       <c r="A65" s="13"/>
       <c r="C65" s="13"/>
     </row>
-    <row r="66" spans="1:3" ht="18.75">
+    <row r="66" spans="1:3" ht="18.3">
       <c r="A66" s="13"/>
       <c r="C66" s="13"/>
     </row>
-    <row r="67" spans="1:3" ht="18.75">
+    <row r="67" spans="1:3" ht="18.3">
       <c r="A67" s="13"/>
       <c r="C67" s="13"/>
     </row>
-    <row r="68" spans="1:3" ht="18.75">
+    <row r="68" spans="1:3" ht="18.3">
       <c r="A68" s="13"/>
       <c r="C68" s="13"/>
     </row>
-    <row r="69" spans="1:3" ht="18.75">
+    <row r="69" spans="1:3" ht="18.3">
       <c r="A69" s="13"/>
       <c r="C69" s="13"/>
     </row>
-    <row r="70" spans="1:3" ht="18.75">
+    <row r="70" spans="1:3" ht="18.3">
       <c r="A70" s="13"/>
       <c r="C70" s="13"/>
     </row>
-    <row r="71" spans="1:3" ht="18.75">
+    <row r="71" spans="1:3" ht="18.3">
       <c r="A71" s="13"/>
       <c r="C71" s="13"/>
     </row>
-    <row r="72" spans="1:3" ht="18.75">
+    <row r="72" spans="1:3" ht="18.3">
       <c r="C72" s="13"/>
     </row>
-    <row r="73" spans="1:3" ht="18.75">
+    <row r="73" spans="1:3" ht="18.3">
       <c r="C73" s="13"/>
     </row>
-    <row r="74" spans="1:3" ht="18.75">
+    <row r="74" spans="1:3" ht="18.3">
       <c r="C74" s="13"/>
     </row>
-    <row r="75" spans="1:3" ht="18.75">
+    <row r="75" spans="1:3" ht="18.3">
       <c r="C75" s="13"/>
     </row>
-    <row r="76" spans="1:3" ht="18.75">
+    <row r="76" spans="1:3" ht="18.3">
       <c r="C76" s="13"/>
     </row>
   </sheetData>

</xml_diff>